<commit_message>
1. Update api routes 2. Update database schema
</commit_message>
<xml_diff>
--- a/Materials/API_Routes_v1.xlsx
+++ b/Materials/API_Routes_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Desktop\Next Bootcamp\Project\next-project\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F928D816-BABC-48B9-A3AA-A050D6032FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348D2452-2161-4D09-A405-305D43FF4EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{0C71E60E-8DA8-4520-89B9-225AD43C425F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>new</t>
   </si>
@@ -169,6 +169,84 @@
   </si>
   <si>
     <t>delete particular lesson</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>list of {id, username, email, profile_pic}</t>
+  </si>
+  <si>
+    <t>{id, username, email, profile_pic}</t>
+  </si>
+  <si>
+    <t>{username, email, password}</t>
+  </si>
+  <si>
+    <t>{username, password}</t>
+  </si>
+  <si>
+    <t>{title, description, owner_id, teach}</t>
+  </si>
+  <si>
+    <t>list of {id, title, description, rating, owner_id, teach}</t>
+  </si>
+  <si>
+    <t>{id, title, description, rating, owner_id, teach}</t>
+  </si>
+  <si>
+    <t>{title, description}</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>get all chats</t>
+  </si>
+  <si>
+    <t>get chats from particular lesson</t>
+  </si>
+  <si>
+    <t>send new chat</t>
+  </si>
+  <si>
+    <t>{lesson_id, user_id, content}</t>
+  </si>
+  <si>
+    <t>list of {id, lesson_id, user_id, content}</t>
+  </si>
+  <si>
+    <t>{id, user_id, content}</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>/chat/create</t>
+  </si>
+  <si>
+    <t>/chat/</t>
+  </si>
+  <si>
+    <t>/chat/:id</t>
+  </si>
+  <si>
+    <t>create request for a lesson</t>
+  </si>
+  <si>
+    <t>{lesson_id, user_id, start_datetime}</t>
+  </si>
+  <si>
+    <t>get all request details</t>
+  </si>
+  <si>
+    <t>get particular request detail</t>
+  </si>
+  <si>
+    <t>{id, lesson_id, user_id, start_datetime}</t>
   </si>
 </sst>
 </file>
@@ -568,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C67AC64-0C56-4FE3-873B-9D09A6F4604C}">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,10 +659,12 @@
     <col min="3" max="4" width="8.7265625" style="8"/>
     <col min="5" max="5" width="19.7265625" style="8" customWidth="1"/>
     <col min="6" max="6" width="27.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="8"/>
+    <col min="7" max="7" width="40.7265625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="43.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>40</v>
       </c>
@@ -600,8 +680,14 @@
       <c r="F2" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -615,7 +701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
@@ -626,7 +712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -638,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -650,7 +736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -662,7 +748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>10</v>
@@ -674,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
@@ -685,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
@@ -701,8 +787,11 @@
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
@@ -716,10 +805,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -735,8 +824,11 @@
       <c r="F14" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -750,8 +842,11 @@
       <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H15" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>6</v>
@@ -765,8 +860,11 @@
       <c r="F16" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H16" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>10</v>
@@ -781,7 +879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
@@ -795,7 +893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
@@ -811,8 +909,11 @@
       <c r="F20" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
@@ -825,8 +926,11 @@
       <c r="F21" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H21" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
@@ -839,8 +943,11 @@
       <c r="F22" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H22" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C23" s="5" t="s">
         <v>10</v>
       </c>
@@ -853,8 +960,11 @@
       <c r="F23" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C24" s="5" t="s">
         <v>11</v>
       </c>
@@ -866,6 +976,145 @@
       </c>
       <c r="F24" s="8" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>